<commit_message>
petite modifs avant vérification mentor
</commit_message>
<xml_diff>
--- a/Aviles_Bastien_1_code_032022/recommandation p5.xlsx
+++ b/Aviles_Bastien_1_code_032022/recommandation p5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bastienaviles/Documents/openclassrooms/projet 5/P5-Openclassroom-Kanap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bastienaviles/Documents/openclassrooms/projet 5/P5-Openclassroom-Kanap/Aviles_Bastien_1_code_032022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52418482-8EDF-4C4A-852F-40D04F45D89B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B045FAF-AFDD-024D-87AE-B07A814E1835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -46,32 +46,89 @@
     <t>OK / Description erreur</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
-    <t>page index.js</t>
-  </si>
-  <si>
-    <t>fonction getProducts</t>
-  </si>
-  <si>
     <t>Récupération des donnés du serveur</t>
   </si>
   <si>
-    <t xml:space="preserve">affichages des infos </t>
-  </si>
-  <si>
     <t>page products</t>
   </si>
   <si>
-    <t>page cart</t>
+    <t>page scipt.js</t>
+  </si>
+  <si>
+    <t>affichage des produits de l'API</t>
+  </si>
+  <si>
+    <t>fonction getProducts pour récupérer les produits dans l'api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class addNewProductToCart pour construire la nouveau produit à ajouter au panier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction addProductsToHome </t>
+  </si>
+  <si>
+    <t>pour afficher les produits à la page du produit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction addToCart </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pour ajouter tous les produits au panier</t>
+  </si>
+  <si>
+    <t>affichage de tous les produits ajouter au panier</t>
+  </si>
+  <si>
+    <t>on récupère bien les produits et on ajoute leurs liens , id , url , et description. Affichage du produit avec tous ses éléments</t>
+  </si>
+  <si>
+    <t>grâce à la méthode class constructor : on ajoute  l'id , l'image, le nom ,la quantité et la couleur du produit</t>
+  </si>
+  <si>
+    <t>affichage du nouveau produit avec ses éléments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour récupérer l'id , l'url et le nom du produit choisi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">l'utilisateur peut  bien choisir son produit qui contiendra son id , son image et son nom </t>
+  </si>
+  <si>
+    <t>fonction displayMessageSuccessAddToCart</t>
+  </si>
+  <si>
+    <t>Les fonctions  getIdProductAddToCart , getUrlImgProductAddToCart et getNameProductAddToCar</t>
+  </si>
+  <si>
+    <t>affichage du message de succés d'ajout au panier avec le code en dur créer</t>
+  </si>
+  <si>
+    <t>pour afficher un message de confirmation quand l'utilisateur ajoute une produit au panier</t>
+  </si>
+  <si>
+    <t>fonction checkProductExistes</t>
+  </si>
+  <si>
+    <t>pour vérifier si le produit ajouter au panier par l'utilisateur existe déjà dans le panier , et si c'est le cas on incrémente sa quantité</t>
+  </si>
+  <si>
+    <t>affichage du produit selectionné par l'utlisateur ,et incrémentation de sa quantité si le produit existe</t>
+  </si>
+  <si>
+    <t>fonction pressAddToCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage du produit selectionné par l'utlisateur ,dans le local storage  </t>
+  </si>
+  <si>
+    <t>pour ajouter le produit choisi par l'utilisateur , avec son id, image et nom ,au local storage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -95,8 +152,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +201,16 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -348,11 +445,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -399,28 +498,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
     <cellStyle name="Neutre" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -636,10 +746,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -669,16 +779,16 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -686,96 +796,138 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="71" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" ht="52" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="83" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="61" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
@@ -839,18 +991,11 @@
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modif après soutenance sur vérif qu'une bonne couleur est saisie
</commit_message>
<xml_diff>
--- a/Aviles_Bastien_1_code_032022/recommandation p5.xlsx
+++ b/Aviles_Bastien_1_code_032022/recommandation p5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bastienaviles/Documents/openclassrooms/projet 5/P5-Openclassroom-Kanap/Aviles_Bastien_1_code_032022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B045FAF-AFDD-024D-87AE-B07A814E1835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA63D1A6-E94B-E944-8F73-4FFDA526C6B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -115,20 +115,119 @@
     <t>affichage du produit selectionné par l'utlisateur ,et incrémentation de sa quantité si le produit existe</t>
   </si>
   <si>
-    <t>fonction pressAddToCart</t>
-  </si>
-  <si>
     <t xml:space="preserve">affichage du produit selectionné par l'utlisateur ,dans le local storage  </t>
   </si>
   <si>
     <t>pour ajouter le produit choisi par l'utilisateur , avec son id, image et nom ,au local storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les fonctions  displayMessageErrorColor et displayMessageErrorQuantity </t>
+  </si>
+  <si>
+    <t>pour afficher un message d'erreur si la quantité ou la couleurs n'est pas saisie par l'utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage d'un message d'erreur codé en dur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">page carts </t>
+  </si>
+  <si>
+    <t>fonction verifLocalStorage</t>
+  </si>
+  <si>
+    <t>fonction pressAddToCart+D12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour vérifier si le local storage n'est pas vide ce qui permettra à l'utilisateur de retrouver son panier lors de sa session </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage du panier vide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour afficher le total du prix des produits choisi par l'utilisateur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage de la quantité total des produits selectionnés dans le panier </t>
+  </si>
+  <si>
+    <t>fonction totalQuantityCart puis fetch http://localhost:3000/api/products/"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage du prix dans le panier du seul produit selectionné parl'utilisateur </t>
+  </si>
+  <si>
+    <t>pour afficher le prix d'un produit avec une quantité egale à1 selectionné par l'utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour afficher le total du prix d'un produit si quantité est suppérieur à 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage du prix total dans le panier du produit selectionné parl'utilisateur </t>
+  </si>
+  <si>
+    <t>fonction priceOneProduct (meme procédé pour la fonction qui gère la quantité d'un produit : quantityOneProduct)</t>
+  </si>
+  <si>
+    <t>fonction totalPriceOneProduit (même procédé pour la fonction qui gère la quantité d'un produit : totalPriceOneProduit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour calculer le total des quantités des produits choisi par l'utilisateur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">suppression du produit selectionné par l'utilisateur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction deleteButton </t>
+  </si>
+  <si>
+    <t>pour la suppression d'un produit du panier quand l'utilisateur clique sur le bouton "supprimer"</t>
+  </si>
+  <si>
+    <t>les fonctions : regExpText , regExpAddress et regExpEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour que l'utilisateur remplisse correctement les champs demandés </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage des éexpression demandées si correctement saisies par l'utilisateur sinon affichage des messages d'erreurs </t>
+  </si>
+  <si>
+    <t>fonction errorsInput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permet à l'utilisateur d'avoir un message d'erreur si il oubli  de remplir un champ ou si il y a une erreur avant de valider sa commande </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage d'un message d'erreur en dur </t>
+  </si>
+  <si>
+    <t>page carts</t>
+  </si>
+  <si>
+    <t>fonction sendOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permet àl'utilisateur d'obtenir un numéro de commande </t>
+  </si>
+  <si>
+    <t xml:space="preserve">permet àl'utilisateur de valider sa commander </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage d'un message de validation de commande en dur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage en dur du numéro de commande </t>
+  </si>
+  <si>
+    <t>fonction validOrder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -167,20 +266,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="16"/>
       <color rgb="FF9C5700"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="16"/>
       <color rgb="FF006100"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
     </font>
   </fonts>
   <fills count="6">
@@ -212,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -382,64 +513,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -451,7 +524,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -474,55 +547,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -748,8 +809,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -775,20 +836,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -796,33 +857,33 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -830,16 +891,16 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -847,155 +908,243 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="24" t="s">
+    <row r="8" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="83" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="21" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="61" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+      <c r="D11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="76" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="73" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>